<commit_message>
add note with assumptions about zanzibar
</commit_message>
<xml_diff>
--- a/global-summary/data_dictionary.xlsx
+++ b/global-summary/data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/NAPHS-data/global-summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3412D6CF-9EC7-A74C-80CE-704081651D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C569A91-1A93-3B44-83DF-EFAEEDA39325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>From the CIA World Factbook: "Codes for the Representation of Names of Countries (ISO 3166) is prepared by the International Organization for Standardization. ISO 3166 includes two- and three-character alphabetic codes and three-digit numeric codes that may be needed for activities involving exchange of data with international organizations that have adopted that standard. Except for the numeric codes, ISO 3166 codes have been adopted in the US as FIPS 104-1: American National Standard Codes for the Representation of Names of Countries, Dependencies, and Areas of Special Sovereignty for Information Interchange."</t>
   </si>
   <si>
-    <t>From the CIA World Factbook: "The Geopolitical Entities, Names, and Codes (GENC) Standard is the US Government-approved profile of names of countries and country subdivisions. Based on ISO 3166 Codes for the representation of names of countries and their subdivisions, it specifies an authoritative set of country codes and names for use by the Federal Government for information exchange. GENC uses ISO 3166 (Parts 1 and 2) names and code elements wherever possible, with modifications only where necessary to comply with US law and US Government recognition policy. This profile addresses unique US Government requirements for: restrictions in recognition of the national sovereignty of a country; identification and recognition of geopolitical entities not included in ISO 3166; and the use of names of countries and country subdivisions that have been approved by the US Board on Geographic Names. "</t>
-  </si>
-  <si>
     <t>country.tsv</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Boolean (TRUE/FALSE) indicating whether the country published machine-readable (e.g., .csv, .tsv) line-item cost estimate as part of their published National Action Plan for Health Security (NAPHS) as of February 2023, NULL if no NAPHS has been published</t>
+  </si>
+  <si>
+    <t>From the CIA World Factbook: "The Geopolitical Entities, Names, and Codes (GENC) Standard is the US Government-approved profile of names of countries and country subdivisions. Based on ISO 3166 Codes for the representation of names of countries and their subdivisions, it specifies an authoritative set of country codes and names for use by the Federal Government for information exchange. GENC uses ISO 3166 (Parts 1 and 2) names and code elements wherever possible, with modifications only where necessary to comply with US law and US Government recognition policy. This profile addresses unique US Government requirements for: restrictions in recognition of the national sovereignty of a country; identification and recognition of geopolitical entities not included in ISO 3166; and the use of names of countries and country subdivisions that have been approved by the US Board on Geographic Names." Note that Zanzibar is not included because it is not (independently) an IHR member state (see Tanzania). Zanzibar's data were not combined with Tanzania, and were excluded from analysis and summary graphics.</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -555,7 +555,7 @@
     </row>
     <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -564,12 +564,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -583,91 +583,91 @@
     </row>
     <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>